<commit_message>
CSI1101 A2: added more images, finished bib, ready for submission
</commit_message>
<xml_diff>
--- a/year_1/sem_2/CSI1101_computer_security/0b_assignment_2_[22MAY15_0900]/dev/bib_v3.xlsx
+++ b/year_1/sem_2/CSI1101_computer_security/0b_assignment_2_[22MAY15_0900]/dev/bib_v3.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -13,10 +13,491 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <r>
+      <t xml:space="preserve">@pent0thal. (2015). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Another password spotted in the wild... [Twitter post]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved May 16, 2015, from https://twitter.com/pent0thal/status/586284074223984642</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AV-TEST. (2013). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Patch Management Solutions Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved May 16, 2015, from http://www.av-test.org/fileadmin/pdf/avtest_2013-07_patch_management_english.pdf</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AV-TEST. (2014a). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test antivirus software for Windows 7 - December 2014 | AV-TEST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved May 16, 2015, from http://www.av-test.org/en/antivirus/business-windows-client/windows-7/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AV-TEST. (2014b). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test Kaspersky Lab Endpoint Security for Windows 7 | AV-TEST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved May 16, 2015, from http://www.av-test.org/en/antivirus/business-windows-client/windows-7/december-2014/kaspersky-lab-endpoint-security-10.2-145015/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Carrera, E. (2002). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Linux.Devnull</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved May 18, 2015, from https://www.f-secure.com/v-descs/devnull.shtml</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">cohdra. (2005). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>100_7363.JPG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved May 16, 2015, from http://www.morguefile.com/archive/display/41812</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ConceptDraw. (n.d.). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>COMPUTER-AND-NETWORKS-Active-Directory-Domain-Services-diagram-Sample.png (1115×788)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved May 16, 2015, from http://www.conceptdraw.com/solution-park/resource/images/solutions/active-directory-diagrams/COMPUTER-AND-NETWORKS-Active-Directory-Domain-Services-diagram-Sample.png</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">jppi. (2007). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sw_locked_gate.jpg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved May 16, 2015, from http://www.morguefile.com/archive/display/129268</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Microsoft. (n.d.). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Screen Saver timeout</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved May 14, 2015, from https://technet.microsoft.com/en-us/library/cc961876.aspx</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Microsoft. (2005a). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Apply or modify password policy: Logon and Authentication</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved May 14, 2015, from https://technet.microsoft.com/en-au/library/cc781633(v=ws.10).aspx?f=255&amp;MSPPError=-2147217396#BKMK_3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Microsoft. (2005b). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Assign user rights to a group in Active Directory: Active Directory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved May 14, 2015, from https://technet.microsoft.com/en-au/library/cc786658(v=ws.10).aspx</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Microsoft. (2007a). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Active Directory Domain Services Overview</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved May 18, 2015, from https://technet.microsoft.com/en-us/library/cc731053(WS.10).aspx</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Microsoft. (2007b). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Configure UAC settings via policy - Microsoft Reduce Customer Effort Center - Site Home - TechNet Blogs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved May 14, 2015, from http://blogs.technet.com/b/asiasupp/archive/2007/02/08/configure-uac-settings-via-policy.aspx</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Microsoft. (2012). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Password must meet complexity requirements</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved May 14, 2015, from https://technet.microsoft.com/en-us/library/hh994562(v=ws.10).aspx</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pietroforte, M. (2006). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The second worst new feature of Windows Vista - 4sysops</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved May 18, 2015, from https://4sysops.com/archives/the-second-worst-new-feature-of-windows-vista/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Oliver, J., &amp; Snowden, E. [LastWeekTonight]. (2015). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Last Week Tonight with John Oliver: Edward Snowden on Passwords</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved May 6, 2015, from https://www.youtube.com/watch?v=yzGzB-yYKcc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Kaspersky Lab. (2013b). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>About KASPERSKY ENDPOINT SECURITY FOR BUSINESS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved May 16, 2015, from http://media.kaspersky.com/en/business-security/endpoint-overview.pdf</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Kaspersky Lab [Kaspersky Lab]. (2013c). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Introducing Kaspersky Endpoint Security for Business (Advanced)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved May 16, 2015, from https://www.youtube.com/watch?v=ctYWZxSVE-s</t>
+    </r>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -44,14 +525,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +591,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +626,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +834,112 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:A18">
+    <sortCondition ref="A4"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>